<commit_message>
Validation for sum made
</commit_message>
<xml_diff>
--- a/Data/Exports/Фактура 11.pdf_1-1.xlsx
+++ b/Data/Exports/Фактура 11.pdf_1-1.xlsx
@@ -97,7 +97,7 @@
     <x:t>table</x:t>
   </x:si>
   <x:si>
-    <x:t>0.7170978</x:t>
+    <x:t>0.7170979</x:t>
   </x:si>
   <x:si>
     <x:t>11.00</x:t>
@@ -156,13 +156,13 @@
     <x:t>0.8789426</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9777557</x:t>
+    <x:t>0.9777555</x:t>
   </x:si>
   <x:si>
     <x:t>грав</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9447877</x:t>
+    <x:t>0.9447879</x:t>
   </x:si>
   <x:si>
     <x:t>60.00</x:t>
@@ -192,13 +192,13 @@
     <x:t>16.00</x:t>
   </x:si>
   <x:si>
-    <x:t>0.9322237</x:t>
+    <x:t>0.9322239</x:t>
   </x:si>
   <x:si>
     <x:t>15</x:t>
   </x:si>
   <x:si>
-    <x:t>0.8371121</x:t>
+    <x:t>0.8371122</x:t>
   </x:si>
   <x:si>
     <x:t>240.00</x:t>
@@ -283,7 +283,31 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="8">
+  <x:cellStyleXfs count="16">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>

</xml_diff>